<commit_message>
Clean up of files
</commit_message>
<xml_diff>
--- a/PyBank/PyBank_Resources_budget_data.xlsx
+++ b/PyBank/PyBank_Resources_budget_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2562e37d3483ba37/Documents/ASU FinTech/python-homework/PyBank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9B86481A-59EC-4E1E-A074-B477FAD585DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:40009_{9B86481A-59EC-4E1E-A074-B477FAD585DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{01163D80-108B-49BA-8A29-100D47B407E1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Homework_Homework2_Instructions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -49,12 +59,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -544,21 +554,23 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -915,14 +927,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -960,6 +976,14 @@
       <c r="B3" s="5">
         <v>984655</v>
       </c>
+      <c r="C3" s="8">
+        <f>B3-B2</f>
+        <v>116771</v>
+      </c>
+      <c r="D3" s="8">
+        <f t="shared" ref="D3:D4" si="0">C3+D2</f>
+        <v>116771</v>
+      </c>
       <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
@@ -975,6 +999,14 @@
       <c r="B4" s="5">
         <v>322013</v>
       </c>
+      <c r="C4" s="8">
+        <f t="shared" ref="C4:C67" si="1">B4-B3</f>
+        <v>-662642</v>
+      </c>
+      <c r="D4" s="8">
+        <f>C4+D3</f>
+        <v>-545871</v>
+      </c>
       <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
@@ -990,15 +1022,23 @@
       <c r="B5" s="5">
         <v>-69417</v>
       </c>
+      <c r="C5" s="8">
+        <f t="shared" si="1"/>
+        <v>-391430</v>
+      </c>
+      <c r="D5" s="8">
+        <f>C5+D4</f>
+        <v>-937301</v>
+      </c>
       <c r="G5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="5">
-        <f>MAX($B$2:$B$87)</f>
-        <v>1170593</v>
+        <f>MAX($C$2:$C$87)</f>
+        <v>1926159</v>
       </c>
       <c r="I5" s="1">
-        <f>_xlfn.XLOOKUP(H5,B2:B87,A2:A87)</f>
+        <f>_xlfn.XLOOKUP(H5,C2:C87,A2:A87)</f>
         <v>40940</v>
       </c>
       <c r="J5" s="1"/>
@@ -1010,15 +1050,23 @@
       <c r="B6" s="5">
         <v>310503</v>
       </c>
+      <c r="C6" s="8">
+        <f t="shared" si="1"/>
+        <v>379920</v>
+      </c>
+      <c r="D6" s="8">
+        <f>C6+D5</f>
+        <v>-557381</v>
+      </c>
       <c r="G6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H6" s="5">
-        <f>MIN($B$2:$B$87)</f>
-        <v>-1196225</v>
+        <f>MIN($C$2:$C$87)</f>
+        <v>-2196167</v>
       </c>
       <c r="I6" s="1">
-        <f>_xlfn.XLOOKUP(H6,B3:B88,A3:A88)</f>
+        <f>_xlfn.XLOOKUP(H6,C3:C88,A3:A88)</f>
         <v>41518</v>
       </c>
     </row>
@@ -1029,6 +1077,14 @@
       <c r="B7" s="5">
         <v>522857</v>
       </c>
+      <c r="C7" s="8">
+        <f t="shared" si="1"/>
+        <v>212354</v>
+      </c>
+      <c r="D7" s="8">
+        <f>C7+D6</f>
+        <v>-345027</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -1037,6 +1093,14 @@
       <c r="B8" s="5">
         <v>1033096</v>
       </c>
+      <c r="C8" s="8">
+        <f t="shared" si="1"/>
+        <v>510239</v>
+      </c>
+      <c r="D8" s="8">
+        <f>C8+D7</f>
+        <v>165212</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -1045,6 +1109,14 @@
       <c r="B9" s="5">
         <v>604885</v>
       </c>
+      <c r="C9" s="8">
+        <f t="shared" si="1"/>
+        <v>-428211</v>
+      </c>
+      <c r="D9" s="8">
+        <f>C9+D8</f>
+        <v>-262999</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1053,6 +1125,14 @@
       <c r="B10" s="5">
         <v>-216386</v>
       </c>
+      <c r="C10" s="8">
+        <f t="shared" si="1"/>
+        <v>-821271</v>
+      </c>
+      <c r="D10" s="8">
+        <f>C10+D9</f>
+        <v>-1084270</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1061,6 +1141,14 @@
       <c r="B11" s="5">
         <v>477532</v>
       </c>
+      <c r="C11" s="8">
+        <f t="shared" si="1"/>
+        <v>693918</v>
+      </c>
+      <c r="D11" s="8">
+        <f>C11+D10</f>
+        <v>-390352</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1069,6 +1157,14 @@
       <c r="B12" s="5">
         <v>893810</v>
       </c>
+      <c r="C12" s="8">
+        <f t="shared" si="1"/>
+        <v>416278</v>
+      </c>
+      <c r="D12" s="8">
+        <f>C12+D11</f>
+        <v>25926</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1077,6 +1173,14 @@
       <c r="B13" s="5">
         <v>-80353</v>
       </c>
+      <c r="C13" s="8">
+        <f t="shared" si="1"/>
+        <v>-974163</v>
+      </c>
+      <c r="D13" s="8">
+        <f t="shared" ref="D6:D69" si="2">C13+D12</f>
+        <v>-948237</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1085,6 +1189,14 @@
       <c r="B14" s="5">
         <v>779806</v>
       </c>
+      <c r="C14" s="8">
+        <f t="shared" si="1"/>
+        <v>860159</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="2"/>
+        <v>-88078</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -1093,6 +1205,14 @@
       <c r="B15" s="5">
         <v>-335203</v>
       </c>
+      <c r="C15" s="8">
+        <f t="shared" si="1"/>
+        <v>-1115009</v>
+      </c>
+      <c r="D15" s="8">
+        <f t="shared" si="2"/>
+        <v>-1203087</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -1101,580 +1221,1175 @@
       <c r="B16" s="5">
         <v>697845</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="8">
+        <f t="shared" si="1"/>
+        <v>1033048</v>
+      </c>
+      <c r="D16" s="8">
+        <f t="shared" si="2"/>
+        <v>-170039</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>40634</v>
       </c>
       <c r="B17" s="5">
         <v>793163</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="8">
+        <f t="shared" si="1"/>
+        <v>95318</v>
+      </c>
+      <c r="D17" s="8">
+        <f t="shared" si="2"/>
+        <v>-74721</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>40664</v>
       </c>
       <c r="B18" s="5">
         <v>485070</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="8">
+        <f t="shared" si="1"/>
+        <v>-308093</v>
+      </c>
+      <c r="D18" s="8">
+        <f t="shared" si="2"/>
+        <v>-382814</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>40695</v>
       </c>
       <c r="B19" s="5">
         <v>584122</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="8">
+        <f t="shared" si="1"/>
+        <v>99052</v>
+      </c>
+      <c r="D19" s="8">
+        <f t="shared" si="2"/>
+        <v>-283762</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>40725</v>
       </c>
       <c r="B20" s="5">
         <v>62729</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="8">
+        <f t="shared" si="1"/>
+        <v>-521393</v>
+      </c>
+      <c r="D20" s="8">
+        <f t="shared" si="2"/>
+        <v>-805155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>40756</v>
       </c>
       <c r="B21" s="5">
         <v>668179</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="8">
+        <f t="shared" si="1"/>
+        <v>605450</v>
+      </c>
+      <c r="D21" s="8">
+        <f t="shared" si="2"/>
+        <v>-199705</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>40787</v>
       </c>
       <c r="B22" s="5">
         <v>899906</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="8">
+        <f t="shared" si="1"/>
+        <v>231727</v>
+      </c>
+      <c r="D22" s="8">
+        <f t="shared" si="2"/>
+        <v>32022</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>40817</v>
       </c>
       <c r="B23" s="5">
         <v>834719</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="8">
+        <f t="shared" si="1"/>
+        <v>-65187</v>
+      </c>
+      <c r="D23" s="8">
+        <f t="shared" si="2"/>
+        <v>-33165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>40848</v>
       </c>
       <c r="B24" s="5">
         <v>132003</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="8">
+        <f t="shared" si="1"/>
+        <v>-702716</v>
+      </c>
+      <c r="D24" s="8">
+        <f t="shared" si="2"/>
+        <v>-735881</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>40878</v>
       </c>
       <c r="B25" s="5">
         <v>309978</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="8">
+        <f t="shared" si="1"/>
+        <v>177975</v>
+      </c>
+      <c r="D25" s="8">
+        <f t="shared" si="2"/>
+        <v>-557906</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>40909</v>
       </c>
       <c r="B26" s="5">
         <v>-755566</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="8">
+        <f t="shared" si="1"/>
+        <v>-1065544</v>
+      </c>
+      <c r="D26" s="8">
+        <f t="shared" si="2"/>
+        <v>-1623450</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>40940</v>
       </c>
       <c r="B27" s="5">
         <v>1170593</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" s="8">
+        <f t="shared" si="1"/>
+        <v>1926159</v>
+      </c>
+      <c r="D27" s="8">
+        <f t="shared" si="2"/>
+        <v>302709</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>40969</v>
       </c>
       <c r="B28" s="5">
         <v>252788</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" s="8">
+        <f t="shared" si="1"/>
+        <v>-917805</v>
+      </c>
+      <c r="D28" s="8">
+        <f t="shared" si="2"/>
+        <v>-615096</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>41000</v>
       </c>
       <c r="B29" s="5">
         <v>1151518</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="8">
+        <f t="shared" si="1"/>
+        <v>898730</v>
+      </c>
+      <c r="D29" s="8">
+        <f t="shared" si="2"/>
+        <v>283634</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>41030</v>
       </c>
       <c r="B30" s="5">
         <v>817256</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="8">
+        <f t="shared" si="1"/>
+        <v>-334262</v>
+      </c>
+      <c r="D30" s="8">
+        <f t="shared" si="2"/>
+        <v>-50628</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>41061</v>
       </c>
       <c r="B31" s="5">
         <v>570757</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" s="8">
+        <f t="shared" si="1"/>
+        <v>-246499</v>
+      </c>
+      <c r="D31" s="8">
+        <f t="shared" si="2"/>
+        <v>-297127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>41091</v>
       </c>
       <c r="B32" s="5">
         <v>506702</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="8">
+        <f t="shared" si="1"/>
+        <v>-64055</v>
+      </c>
+      <c r="D32" s="8">
+        <f t="shared" si="2"/>
+        <v>-361182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>41122</v>
       </c>
       <c r="B33" s="5">
         <v>-1022534</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" s="8">
+        <f t="shared" si="1"/>
+        <v>-1529236</v>
+      </c>
+      <c r="D33" s="8">
+        <f t="shared" si="2"/>
+        <v>-1890418</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>41153</v>
       </c>
       <c r="B34" s="5">
         <v>475062</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" s="8">
+        <f t="shared" si="1"/>
+        <v>1497596</v>
+      </c>
+      <c r="D34" s="8">
+        <f t="shared" si="2"/>
+        <v>-392822</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>41183</v>
       </c>
       <c r="B35" s="5">
         <v>779976</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" s="8">
+        <f t="shared" si="1"/>
+        <v>304914</v>
+      </c>
+      <c r="D35" s="8">
+        <f t="shared" si="2"/>
+        <v>-87908</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>41214</v>
       </c>
       <c r="B36" s="5">
         <v>144175</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" s="8">
+        <f t="shared" si="1"/>
+        <v>-635801</v>
+      </c>
+      <c r="D36" s="8">
+        <f t="shared" si="2"/>
+        <v>-723709</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>41244</v>
       </c>
       <c r="B37" s="5">
         <v>542494</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" s="8">
+        <f t="shared" si="1"/>
+        <v>398319</v>
+      </c>
+      <c r="D37" s="8">
+        <f t="shared" si="2"/>
+        <v>-325390</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>41275</v>
       </c>
       <c r="B38" s="5">
         <v>359333</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" s="8">
+        <f t="shared" si="1"/>
+        <v>-183161</v>
+      </c>
+      <c r="D38" s="8">
+        <f t="shared" si="2"/>
+        <v>-508551</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>41306</v>
       </c>
       <c r="B39" s="5">
         <v>321469</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" s="8">
+        <f t="shared" si="1"/>
+        <v>-37864</v>
+      </c>
+      <c r="D39" s="8">
+        <f t="shared" si="2"/>
+        <v>-546415</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>41334</v>
       </c>
       <c r="B40" s="5">
         <v>67780</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" s="8">
+        <f t="shared" si="1"/>
+        <v>-253689</v>
+      </c>
+      <c r="D40" s="8">
+        <f t="shared" si="2"/>
+        <v>-800104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>41365</v>
       </c>
       <c r="B41" s="5">
         <v>471435</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" s="8">
+        <f t="shared" si="1"/>
+        <v>403655</v>
+      </c>
+      <c r="D41" s="8">
+        <f t="shared" si="2"/>
+        <v>-396449</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41395</v>
       </c>
       <c r="B42" s="5">
         <v>565603</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" s="8">
+        <f t="shared" si="1"/>
+        <v>94168</v>
+      </c>
+      <c r="D42" s="8">
+        <f t="shared" si="2"/>
+        <v>-302281</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41426</v>
       </c>
       <c r="B43" s="5">
         <v>872480</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" s="8">
+        <f t="shared" si="1"/>
+        <v>306877</v>
+      </c>
+      <c r="D43" s="8">
+        <f t="shared" si="2"/>
+        <v>4596</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>41456</v>
       </c>
       <c r="B44" s="5">
         <v>789480</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" s="8">
+        <f t="shared" si="1"/>
+        <v>-83000</v>
+      </c>
+      <c r="D44" s="8">
+        <f t="shared" si="2"/>
+        <v>-78404</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>41487</v>
       </c>
       <c r="B45" s="5">
         <v>999942</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" s="8">
+        <f t="shared" si="1"/>
+        <v>210462</v>
+      </c>
+      <c r="D45" s="8">
+        <f t="shared" si="2"/>
+        <v>132058</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>41518</v>
       </c>
       <c r="B46" s="5">
         <v>-1196225</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" s="8">
+        <f t="shared" si="1"/>
+        <v>-2196167</v>
+      </c>
+      <c r="D46" s="8">
+        <f t="shared" si="2"/>
+        <v>-2064109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>41548</v>
       </c>
       <c r="B47" s="5">
         <v>268997</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" s="8">
+        <f t="shared" si="1"/>
+        <v>1465222</v>
+      </c>
+      <c r="D47" s="8">
+        <f t="shared" si="2"/>
+        <v>-598887</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>41579</v>
       </c>
       <c r="B48" s="5">
         <v>-687986</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" s="8">
+        <f t="shared" si="1"/>
+        <v>-956983</v>
+      </c>
+      <c r="D48" s="8">
+        <f t="shared" si="2"/>
+        <v>-1555870</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>41609</v>
       </c>
       <c r="B49" s="5">
         <v>1150461</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" s="8">
+        <f t="shared" si="1"/>
+        <v>1838447</v>
+      </c>
+      <c r="D49" s="8">
+        <f t="shared" si="2"/>
+        <v>282577</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>41640</v>
       </c>
       <c r="B50" s="5">
         <v>682458</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" s="8">
+        <f t="shared" si="1"/>
+        <v>-468003</v>
+      </c>
+      <c r="D50" s="8">
+        <f t="shared" si="2"/>
+        <v>-185426</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>41671</v>
       </c>
       <c r="B51" s="5">
         <v>617856</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" s="8">
+        <f t="shared" si="1"/>
+        <v>-64602</v>
+      </c>
+      <c r="D51" s="8">
+        <f t="shared" si="2"/>
+        <v>-250028</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>41699</v>
       </c>
       <c r="B52" s="5">
         <v>824098</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" s="8">
+        <f t="shared" si="1"/>
+        <v>206242</v>
+      </c>
+      <c r="D52" s="8">
+        <f t="shared" si="2"/>
+        <v>-43786</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>41730</v>
       </c>
       <c r="B53" s="5">
         <v>581943</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" s="8">
+        <f t="shared" si="1"/>
+        <v>-242155</v>
+      </c>
+      <c r="D53" s="8">
+        <f t="shared" si="2"/>
+        <v>-285941</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>41760</v>
       </c>
       <c r="B54" s="5">
         <v>132864</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" s="8">
+        <f t="shared" si="1"/>
+        <v>-449079</v>
+      </c>
+      <c r="D54" s="8">
+        <f t="shared" si="2"/>
+        <v>-735020</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>41791</v>
       </c>
       <c r="B55" s="5">
         <v>448062</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" s="8">
+        <f t="shared" si="1"/>
+        <v>315198</v>
+      </c>
+      <c r="D55" s="8">
+        <f t="shared" si="2"/>
+        <v>-419822</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>41821</v>
       </c>
       <c r="B56" s="5">
         <v>689161</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" s="8">
+        <f t="shared" si="1"/>
+        <v>241099</v>
+      </c>
+      <c r="D56" s="8">
+        <f t="shared" si="2"/>
+        <v>-178723</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>41852</v>
       </c>
       <c r="B57" s="5">
         <v>800701</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" s="8">
+        <f t="shared" si="1"/>
+        <v>111540</v>
+      </c>
+      <c r="D57" s="8">
+        <f t="shared" si="2"/>
+        <v>-67183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>41883</v>
       </c>
       <c r="B58" s="5">
         <v>1166643</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" s="8">
+        <f t="shared" si="1"/>
+        <v>365942</v>
+      </c>
+      <c r="D58" s="8">
+        <f t="shared" si="2"/>
+        <v>298759</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>41913</v>
       </c>
       <c r="B59" s="5">
         <v>947333</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" s="8">
+        <f t="shared" si="1"/>
+        <v>-219310</v>
+      </c>
+      <c r="D59" s="8">
+        <f t="shared" si="2"/>
+        <v>79449</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>41944</v>
       </c>
       <c r="B60" s="5">
         <v>578668</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" s="8">
+        <f t="shared" si="1"/>
+        <v>-368665</v>
+      </c>
+      <c r="D60" s="8">
+        <f t="shared" si="2"/>
+        <v>-289216</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>41974</v>
       </c>
       <c r="B61" s="5">
         <v>988505</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" s="8">
+        <f t="shared" si="1"/>
+        <v>409837</v>
+      </c>
+      <c r="D61" s="8">
+        <f t="shared" si="2"/>
+        <v>120621</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>42005</v>
       </c>
       <c r="B62" s="5">
         <v>1139715</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62" s="8">
+        <f t="shared" si="1"/>
+        <v>151210</v>
+      </c>
+      <c r="D62" s="8">
+        <f t="shared" si="2"/>
+        <v>271831</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>42036</v>
       </c>
       <c r="B63" s="5">
         <v>1029471</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63" s="8">
+        <f t="shared" si="1"/>
+        <v>-110244</v>
+      </c>
+      <c r="D63" s="8">
+        <f t="shared" si="2"/>
+        <v>161587</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>42064</v>
       </c>
       <c r="B64" s="5">
         <v>687533</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64" s="8">
+        <f t="shared" si="1"/>
+        <v>-341938</v>
+      </c>
+      <c r="D64" s="8">
+        <f t="shared" si="2"/>
+        <v>-180351</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>42095</v>
       </c>
       <c r="B65" s="5">
         <v>-524626</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" s="8">
+        <f t="shared" si="1"/>
+        <v>-1212159</v>
+      </c>
+      <c r="D65" s="8">
+        <f t="shared" si="2"/>
+        <v>-1392510</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>42125</v>
       </c>
       <c r="B66" s="5">
         <v>158620</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66" s="8">
+        <f t="shared" si="1"/>
+        <v>683246</v>
+      </c>
+      <c r="D66" s="8">
+        <f t="shared" si="2"/>
+        <v>-709264</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>42156</v>
       </c>
       <c r="B67" s="5">
         <v>87795</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" s="8">
+        <f t="shared" si="1"/>
+        <v>-70825</v>
+      </c>
+      <c r="D67" s="8">
+        <f t="shared" si="2"/>
+        <v>-780089</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>42186</v>
       </c>
       <c r="B68" s="5">
         <v>423389</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" s="8">
+        <f t="shared" ref="C68:C87" si="3">B68-B67</f>
+        <v>335594</v>
+      </c>
+      <c r="D68" s="8">
+        <f t="shared" si="2"/>
+        <v>-444495</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>42217</v>
       </c>
       <c r="B69" s="5">
         <v>840723</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69" s="8">
+        <f t="shared" si="3"/>
+        <v>417334</v>
+      </c>
+      <c r="D69" s="8">
+        <f t="shared" si="2"/>
+        <v>-27161</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>42248</v>
       </c>
       <c r="B70" s="5">
         <v>568529</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70" s="8">
+        <f t="shared" si="3"/>
+        <v>-272194</v>
+      </c>
+      <c r="D70" s="8">
+        <f t="shared" ref="D70:D87" si="4">C70+D69</f>
+        <v>-299355</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>42278</v>
       </c>
       <c r="B71" s="5">
         <v>332067</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" s="8">
+        <f t="shared" si="3"/>
+        <v>-236462</v>
+      </c>
+      <c r="D71" s="8">
+        <f t="shared" si="4"/>
+        <v>-535817</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>42309</v>
       </c>
       <c r="B72" s="5">
         <v>989499</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72" s="8">
+        <f t="shared" si="3"/>
+        <v>657432</v>
+      </c>
+      <c r="D72" s="8">
+        <f t="shared" si="4"/>
+        <v>121615</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>42339</v>
       </c>
       <c r="B73" s="5">
         <v>778237</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73" s="8">
+        <f t="shared" si="3"/>
+        <v>-211262</v>
+      </c>
+      <c r="D73" s="8">
+        <f t="shared" si="4"/>
+        <v>-89647</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>42370</v>
       </c>
       <c r="B74" s="5">
         <v>650000</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74" s="8">
+        <f t="shared" si="3"/>
+        <v>-128237</v>
+      </c>
+      <c r="D74" s="8">
+        <f t="shared" si="4"/>
+        <v>-217884</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>42401</v>
       </c>
       <c r="B75" s="5">
         <v>-1100387</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75" s="8">
+        <f t="shared" si="3"/>
+        <v>-1750387</v>
+      </c>
+      <c r="D75" s="8">
+        <f t="shared" si="4"/>
+        <v>-1968271</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>42430</v>
       </c>
       <c r="B76" s="5">
         <v>-174946</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76" s="8">
+        <f t="shared" si="3"/>
+        <v>925441</v>
+      </c>
+      <c r="D76" s="8">
+        <f t="shared" si="4"/>
+        <v>-1042830</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>42461</v>
       </c>
       <c r="B77" s="5">
         <v>757143</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77" s="8">
+        <f t="shared" si="3"/>
+        <v>932089</v>
+      </c>
+      <c r="D77" s="8">
+        <f t="shared" si="4"/>
+        <v>-110741</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>42491</v>
       </c>
       <c r="B78" s="5">
         <v>445709</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78" s="8">
+        <f t="shared" si="3"/>
+        <v>-311434</v>
+      </c>
+      <c r="D78" s="8">
+        <f t="shared" si="4"/>
+        <v>-422175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>42522</v>
       </c>
       <c r="B79" s="5">
         <v>712961</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79" s="8">
+        <f t="shared" si="3"/>
+        <v>267252</v>
+      </c>
+      <c r="D79" s="8">
+        <f t="shared" si="4"/>
+        <v>-154923</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>42552</v>
       </c>
       <c r="B80" s="5">
         <v>-1163797</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80" s="8">
+        <f t="shared" si="3"/>
+        <v>-1876758</v>
+      </c>
+      <c r="D80" s="8">
+        <f t="shared" si="4"/>
+        <v>-2031681</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>42583</v>
       </c>
       <c r="B81" s="5">
         <v>569899</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81" s="8">
+        <f t="shared" si="3"/>
+        <v>1733696</v>
+      </c>
+      <c r="D81" s="8">
+        <f t="shared" si="4"/>
+        <v>-297985</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>42614</v>
       </c>
       <c r="B82" s="5">
         <v>768450</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82" s="8">
+        <f t="shared" si="3"/>
+        <v>198551</v>
+      </c>
+      <c r="D82" s="8">
+        <f t="shared" si="4"/>
+        <v>-99434</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>42644</v>
       </c>
       <c r="B83" s="5">
         <v>102685</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83" s="8">
+        <f t="shared" si="3"/>
+        <v>-665765</v>
+      </c>
+      <c r="D83" s="8">
+        <f t="shared" si="4"/>
+        <v>-765199</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>42675</v>
       </c>
       <c r="B84" s="5">
         <v>795914</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84" s="8">
+        <f t="shared" si="3"/>
+        <v>693229</v>
+      </c>
+      <c r="D84" s="8">
+        <f t="shared" si="4"/>
+        <v>-71970</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>42705</v>
       </c>
       <c r="B85" s="5">
         <v>60988</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85" s="8">
+        <f t="shared" si="3"/>
+        <v>-734926</v>
+      </c>
+      <c r="D85" s="8">
+        <f t="shared" si="4"/>
+        <v>-806896</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>42736</v>
       </c>
       <c r="B86" s="5">
         <v>138230</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86" s="8">
+        <f t="shared" si="3"/>
+        <v>77242</v>
+      </c>
+      <c r="D86" s="8">
+        <f t="shared" si="4"/>
+        <v>-729654</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>42767</v>
       </c>
       <c r="B87" s="5">
         <v>671099</v>
+      </c>
+      <c r="C87" s="8">
+        <f>B87-B86</f>
+        <v>532869</v>
+      </c>
+      <c r="D87" s="8">
+        <f>C87+D86</f>
+        <v>-196785</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C88" s="9">
+        <f>AVERAGE(C3:C87)</f>
+        <v>-2315.1176470588234</v>
+      </c>
+      <c r="D88" s="9">
+        <f>D87/85</f>
+        <v>-2315.1176470588234</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C93" s="8">
+        <f>SUM(C3:C87)</f>
+        <v>-196785</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C94" s="9">
+        <f>C93/85</f>
+        <v>-2315.1176470588234</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="I6" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>